<commit_message>
Birth dates errors identification
</commit_message>
<xml_diff>
--- a/data/NewlyCreatedData/Checks/BirthDates.xlsx
+++ b/data/NewlyCreatedData/Checks/BirthDates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\monas\Git\repo\glt\GoldenLionTamarins\data\NewlyCreatedData\Checks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3146DBF7-37B8-470B-8E99-7490B70A3A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F0C7E2-01FA-435A-98B5-988795709810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="488">
   <si>
     <t>Tatoo</t>
   </si>
@@ -1205,9 +1205,6 @@
     <t>01/04/95</t>
   </si>
   <si>
-    <t>00/01/00</t>
-  </si>
-  <si>
     <t>06/04/91</t>
   </si>
   <si>
@@ -1502,7 +1499,7 @@
     <t>01/07/97</t>
   </si>
   <si>
-    <t>BirthDMY</t>
+    <t>Birth_VR</t>
   </si>
 </sst>
 </file>
@@ -1871,7 +1868,7 @@
   <dimension ref="A1:E316"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,7 +1894,7 @@
         <v>352</v>
       </c>
       <c r="E1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2764,7 +2761,7 @@
         <v>353</v>
       </c>
       <c r="E52" t="s">
-        <v>389</v>
+        <v>353</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2781,7 +2778,7 @@
         <v>33334</v>
       </c>
       <c r="E53" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2798,7 +2795,7 @@
         <v>33482</v>
       </c>
       <c r="E54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2832,7 +2829,7 @@
         <v>35400</v>
       </c>
       <c r="E56" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2849,7 +2846,7 @@
         <v>35400</v>
       </c>
       <c r="E57" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2883,7 +2880,7 @@
         <v>36069</v>
       </c>
       <c r="E59" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2900,7 +2897,7 @@
         <v>36069</v>
       </c>
       <c r="E60" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2917,7 +2914,7 @@
         <v>36434</v>
       </c>
       <c r="E61" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2934,7 +2931,7 @@
         <v>36434</v>
       </c>
       <c r="E62" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2951,7 +2948,7 @@
         <v>33756</v>
       </c>
       <c r="E63" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2968,7 +2965,7 @@
         <v>31625</v>
       </c>
       <c r="E64" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2985,7 +2982,7 @@
         <v>224</v>
       </c>
       <c r="E65" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3002,7 +2999,7 @@
         <v>36708</v>
       </c>
       <c r="E66" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3019,7 +3016,7 @@
         <v>34608</v>
       </c>
       <c r="E67" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3036,7 +3033,7 @@
         <v>34608</v>
       </c>
       <c r="E68" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3053,7 +3050,7 @@
         <v>35004</v>
       </c>
       <c r="E69" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3070,7 +3067,7 @@
         <v>35004</v>
       </c>
       <c r="E70" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3087,7 +3084,7 @@
         <v>35309</v>
       </c>
       <c r="E71" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3104,7 +3101,7 @@
         <v>35309</v>
       </c>
       <c r="E72" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3121,7 +3118,7 @@
         <v>35674</v>
       </c>
       <c r="E73" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3138,7 +3135,7 @@
         <v>35674</v>
       </c>
       <c r="E74" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3155,7 +3152,7 @@
         <v>36130</v>
       </c>
       <c r="E75" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3172,7 +3169,7 @@
         <v>36130</v>
       </c>
       <c r="E76" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3189,7 +3186,7 @@
         <v>36434</v>
       </c>
       <c r="E77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3206,7 +3203,7 @@
         <v>36434</v>
       </c>
       <c r="E78" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3257,7 +3254,7 @@
         <v>37165</v>
       </c>
       <c r="E81" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3274,7 +3271,7 @@
         <v>37165</v>
       </c>
       <c r="E82" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3291,7 +3288,7 @@
         <v>33270</v>
       </c>
       <c r="E83" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3308,7 +3305,7 @@
         <v>33329</v>
       </c>
       <c r="E84" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3325,7 +3322,7 @@
         <v>33329</v>
       </c>
       <c r="E85" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3342,7 +3339,7 @@
         <v>36272</v>
       </c>
       <c r="E86" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3410,7 +3407,7 @@
         <v>37165</v>
       </c>
       <c r="E90" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3427,7 +3424,7 @@
         <v>37165</v>
       </c>
       <c r="E91" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3461,7 +3458,7 @@
         <v>32721</v>
       </c>
       <c r="E93" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3512,7 +3509,7 @@
         <v>36495</v>
       </c>
       <c r="E96" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3529,7 +3526,7 @@
         <v>36495</v>
       </c>
       <c r="E97" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3563,7 +3560,7 @@
         <v>31822</v>
       </c>
       <c r="E99" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3580,7 +3577,7 @@
         <v>33520</v>
       </c>
       <c r="E100" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3597,7 +3594,7 @@
         <v>34020</v>
       </c>
       <c r="E101" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3614,7 +3611,7 @@
         <v>34020</v>
       </c>
       <c r="E102" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3631,7 +3628,7 @@
         <v>32478</v>
       </c>
       <c r="E103" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3648,7 +3645,7 @@
         <v>33158</v>
       </c>
       <c r="E104" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3665,7 +3662,7 @@
         <v>33158</v>
       </c>
       <c r="E105" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3682,7 +3679,7 @@
         <v>33520</v>
       </c>
       <c r="E106" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3699,7 +3696,7 @@
         <v>33257</v>
       </c>
       <c r="E107" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3716,7 +3713,7 @@
         <v>34608</v>
       </c>
       <c r="E108" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3801,7 +3798,7 @@
         <v>234</v>
       </c>
       <c r="E113" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3818,7 +3815,7 @@
         <v>234</v>
       </c>
       <c r="E114" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3886,7 +3883,7 @@
         <v>36100</v>
       </c>
       <c r="E118" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3903,7 +3900,7 @@
         <v>36100</v>
       </c>
       <c r="E119" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3954,7 +3951,7 @@
         <v>36708</v>
       </c>
       <c r="E122" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4005,7 +4002,7 @@
         <v>33628</v>
       </c>
       <c r="E125" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4022,7 +4019,7 @@
         <v>34001</v>
       </c>
       <c r="E126" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4039,7 +4036,7 @@
         <v>34608</v>
       </c>
       <c r="E127" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4056,7 +4053,7 @@
         <v>34608</v>
       </c>
       <c r="E128" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4073,7 +4070,7 @@
         <v>34881</v>
       </c>
       <c r="E129" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4107,7 +4104,7 @@
         <v>36708</v>
       </c>
       <c r="E131" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4124,7 +4121,7 @@
         <v>36708</v>
       </c>
       <c r="E132" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4141,7 +4138,7 @@
         <v>34881</v>
       </c>
       <c r="E133" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4158,7 +4155,7 @@
         <v>34881</v>
       </c>
       <c r="E134" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4175,7 +4172,7 @@
         <v>34881</v>
       </c>
       <c r="E135" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4192,7 +4189,7 @@
         <v>35278</v>
       </c>
       <c r="E136" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4209,7 +4206,7 @@
         <v>35643</v>
       </c>
       <c r="E137" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4226,7 +4223,7 @@
         <v>35643</v>
       </c>
       <c r="E138" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4243,7 +4240,7 @@
         <v>35643</v>
       </c>
       <c r="E139" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4345,7 +4342,7 @@
         <v>35348</v>
       </c>
       <c r="E145" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4362,7 +4359,7 @@
         <v>35348</v>
       </c>
       <c r="E146" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4379,7 +4376,7 @@
         <v>35711</v>
       </c>
       <c r="E147" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4396,7 +4393,7 @@
         <v>35711</v>
       </c>
       <c r="E148" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4413,7 +4410,7 @@
         <v>36065</v>
       </c>
       <c r="E149" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4430,7 +4427,7 @@
         <v>36065</v>
       </c>
       <c r="E150" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4447,7 +4444,7 @@
         <v>36413</v>
       </c>
       <c r="E151" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4464,7 +4461,7 @@
         <v>36413</v>
       </c>
       <c r="E152" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4549,7 +4546,7 @@
         <v>37165</v>
       </c>
       <c r="E157" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4566,7 +4563,7 @@
         <v>37165</v>
       </c>
       <c r="E158" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4583,7 +4580,7 @@
         <v>34339</v>
       </c>
       <c r="E159" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4600,7 +4597,7 @@
         <v>34339</v>
       </c>
       <c r="E160" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4617,7 +4614,7 @@
         <v>34620</v>
       </c>
       <c r="E161" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4668,7 +4665,7 @@
         <v>36404</v>
       </c>
       <c r="E164" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4685,7 +4682,7 @@
         <v>36557</v>
       </c>
       <c r="E165" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -4702,7 +4699,7 @@
         <v>36557</v>
       </c>
       <c r="E166" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4753,7 +4750,7 @@
         <v>37165</v>
       </c>
       <c r="E169" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4770,7 +4767,7 @@
         <v>37165</v>
       </c>
       <c r="E170" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4804,7 +4801,7 @@
         <v>34972</v>
       </c>
       <c r="E172" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4821,7 +4818,7 @@
         <v>34972</v>
       </c>
       <c r="E173" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4838,7 +4835,7 @@
         <v>35734</v>
       </c>
       <c r="E174" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4855,7 +4852,7 @@
         <v>35704</v>
       </c>
       <c r="E175" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4872,7 +4869,7 @@
         <v>36039</v>
       </c>
       <c r="E176" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -4889,7 +4886,7 @@
         <v>36039</v>
       </c>
       <c r="E177" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4906,7 +4903,7 @@
         <v>36404</v>
       </c>
       <c r="E178" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -4957,7 +4954,7 @@
         <v>33909</v>
       </c>
       <c r="E181" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -4974,7 +4971,7 @@
         <v>33140</v>
       </c>
       <c r="E182" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5008,7 +5005,7 @@
         <v>36178</v>
       </c>
       <c r="E184" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5025,7 +5022,7 @@
         <v>36178</v>
       </c>
       <c r="E185" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -5042,7 +5039,7 @@
         <v>181</v>
       </c>
       <c r="E186" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5059,7 +5056,7 @@
         <v>181</v>
       </c>
       <c r="E187" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -5127,7 +5124,7 @@
         <v>36923</v>
       </c>
       <c r="E191" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5144,7 +5141,7 @@
         <v>36923</v>
       </c>
       <c r="E192" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5161,7 +5158,7 @@
         <v>33695</v>
       </c>
       <c r="E193" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5178,7 +5175,7 @@
         <v>35217</v>
       </c>
       <c r="E194" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -5195,7 +5192,7 @@
         <v>35217</v>
       </c>
       <c r="E195" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5212,7 +5209,7 @@
         <v>35519</v>
       </c>
       <c r="E196" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -5229,7 +5226,7 @@
         <v>35519</v>
       </c>
       <c r="E197" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -5246,7 +5243,7 @@
         <v>36045</v>
       </c>
       <c r="E198" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -5263,7 +5260,7 @@
         <v>36045</v>
       </c>
       <c r="E199" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -5280,7 +5277,7 @@
         <v>36045</v>
       </c>
       <c r="E200" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5297,7 +5294,7 @@
         <v>36045</v>
       </c>
       <c r="E201" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -5314,7 +5311,7 @@
         <v>36045</v>
       </c>
       <c r="E202" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5331,7 +5328,7 @@
         <v>36178</v>
       </c>
       <c r="E203" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5348,7 +5345,7 @@
         <v>31472</v>
       </c>
       <c r="E204" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5365,7 +5362,7 @@
         <v>32118</v>
       </c>
       <c r="E205" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -5382,7 +5379,7 @@
         <v>37012</v>
       </c>
       <c r="E206" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -5399,7 +5396,7 @@
         <v>37012</v>
       </c>
       <c r="E207" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5416,7 +5413,7 @@
         <v>35777</v>
       </c>
       <c r="E208" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5433,7 +5430,7 @@
         <v>36069</v>
       </c>
       <c r="E209" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5450,7 +5447,7 @@
         <v>36069</v>
       </c>
       <c r="E210" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5467,7 +5464,7 @@
         <v>36404</v>
       </c>
       <c r="E211" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -5484,7 +5481,7 @@
         <v>36404</v>
       </c>
       <c r="E212" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -5535,7 +5532,7 @@
         <v>32174</v>
       </c>
       <c r="E215" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -5569,7 +5566,7 @@
         <v>35035</v>
       </c>
       <c r="E217" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -5586,7 +5583,7 @@
         <v>35035</v>
       </c>
       <c r="E218" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5603,7 +5600,7 @@
         <v>35462</v>
       </c>
       <c r="E219" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -5620,7 +5617,7 @@
         <v>35462</v>
       </c>
       <c r="E220" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -5654,7 +5651,7 @@
         <v>37165</v>
       </c>
       <c r="E222" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5671,7 +5668,7 @@
         <v>37165</v>
       </c>
       <c r="E223" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5688,7 +5685,7 @@
         <v>32752</v>
       </c>
       <c r="E224" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -5705,7 +5702,7 @@
         <v>32752</v>
       </c>
       <c r="E225" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -5722,7 +5719,7 @@
         <v>33899</v>
       </c>
       <c r="E226" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -5739,7 +5736,7 @@
         <v>31423</v>
       </c>
       <c r="E227" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -5756,7 +5753,7 @@
         <v>31423</v>
       </c>
       <c r="E228" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -5773,7 +5770,7 @@
         <v>36065</v>
       </c>
       <c r="E229" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -5790,7 +5787,7 @@
         <v>156</v>
       </c>
       <c r="E230" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -5841,7 +5838,7 @@
         <v>36065</v>
       </c>
       <c r="E233" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -5858,7 +5855,7 @@
         <v>36192</v>
       </c>
       <c r="E234" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -5875,7 +5872,7 @@
         <v>36192</v>
       </c>
       <c r="E235" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -5892,7 +5889,7 @@
         <v>36443</v>
       </c>
       <c r="E236" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -5909,7 +5906,7 @@
         <v>36443</v>
       </c>
       <c r="E237" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -5926,7 +5923,7 @@
         <v>36443</v>
       </c>
       <c r="E238" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -5943,7 +5940,7 @@
         <v>36443</v>
       </c>
       <c r="E239" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -5960,7 +5957,7 @@
         <v>156</v>
       </c>
       <c r="E240" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -5977,7 +5974,7 @@
         <v>156</v>
       </c>
       <c r="E241" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6028,7 +6025,7 @@
         <v>32478</v>
       </c>
       <c r="E244" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6045,7 +6042,7 @@
         <v>31321</v>
       </c>
       <c r="E245" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6062,7 +6059,7 @@
         <v>300</v>
       </c>
       <c r="E246" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6079,7 +6076,7 @@
         <v>300</v>
       </c>
       <c r="E247" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -6130,7 +6127,7 @@
         <v>298</v>
       </c>
       <c r="E250" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6147,7 +6144,7 @@
         <v>304</v>
       </c>
       <c r="E251" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -6164,7 +6161,7 @@
         <v>304</v>
       </c>
       <c r="E252" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -6181,7 +6178,7 @@
         <v>306</v>
       </c>
       <c r="E253" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6198,7 +6195,7 @@
         <v>306</v>
       </c>
       <c r="E254" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -6215,7 +6212,7 @@
         <v>306</v>
       </c>
       <c r="E255" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -6232,7 +6229,7 @@
         <v>306</v>
       </c>
       <c r="E256" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -6249,7 +6246,7 @@
         <v>33878</v>
       </c>
       <c r="E257" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6266,7 +6263,7 @@
         <v>34274</v>
       </c>
       <c r="E258" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -6283,7 +6280,7 @@
         <v>34759</v>
       </c>
       <c r="E259" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6300,7 +6297,7 @@
         <v>34992</v>
       </c>
       <c r="E260" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6317,7 +6314,7 @@
         <v>34992</v>
       </c>
       <c r="E261" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -6334,7 +6331,7 @@
         <v>35342</v>
       </c>
       <c r="E262" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -6351,7 +6348,7 @@
         <v>35342</v>
       </c>
       <c r="E263" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6368,7 +6365,7 @@
         <v>35499</v>
       </c>
       <c r="E264" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -6385,7 +6382,7 @@
         <v>35499</v>
       </c>
       <c r="E265" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -6402,7 +6399,7 @@
         <v>35713</v>
       </c>
       <c r="E266" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -6419,7 +6416,7 @@
         <v>35844</v>
       </c>
       <c r="E267" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -6436,7 +6433,7 @@
         <v>36089</v>
       </c>
       <c r="E268" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -6453,7 +6450,7 @@
         <v>36089</v>
       </c>
       <c r="E269" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -6470,7 +6467,7 @@
         <v>36130</v>
       </c>
       <c r="E270" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6487,7 +6484,7 @@
         <v>36130</v>
       </c>
       <c r="E271" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -6504,7 +6501,7 @@
         <v>36451</v>
       </c>
       <c r="E272" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -6521,7 +6518,7 @@
         <v>36434</v>
       </c>
       <c r="E273" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -6555,7 +6552,7 @@
         <v>33420</v>
       </c>
       <c r="E275" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
@@ -6589,7 +6586,7 @@
         <v>36861</v>
       </c>
       <c r="E277" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -6606,7 +6603,7 @@
         <v>36861</v>
       </c>
       <c r="E278" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -6623,7 +6620,7 @@
         <v>37135</v>
       </c>
       <c r="E279" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
@@ -6640,7 +6637,7 @@
         <v>37165</v>
       </c>
       <c r="E280" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
@@ -6657,7 +6654,7 @@
         <v>37165</v>
       </c>
       <c r="E281" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -6674,7 +6671,7 @@
         <v>34045</v>
       </c>
       <c r="E282" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -6691,7 +6688,7 @@
         <v>34045</v>
       </c>
       <c r="E283" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -6725,7 +6722,7 @@
         <v>33298</v>
       </c>
       <c r="E285" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -6776,7 +6773,7 @@
         <v>34243</v>
       </c>
       <c r="E288" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
@@ -6810,7 +6807,7 @@
         <v>35823</v>
       </c>
       <c r="E290" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -6827,7 +6824,7 @@
         <v>36066</v>
       </c>
       <c r="E291" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -6844,7 +6841,7 @@
         <v>36066</v>
       </c>
       <c r="E292" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -6861,7 +6858,7 @@
         <v>36404</v>
       </c>
       <c r="E293" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -6878,7 +6875,7 @@
         <v>36557</v>
       </c>
       <c r="E294" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -6895,7 +6892,7 @@
         <v>36557</v>
       </c>
       <c r="E295" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -6912,7 +6909,7 @@
         <v>36861</v>
       </c>
       <c r="E296" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -6929,7 +6926,7 @@
         <v>36861</v>
       </c>
       <c r="E297" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
@@ -6946,7 +6943,7 @@
         <v>37196</v>
       </c>
       <c r="E298" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -6963,7 +6960,7 @@
         <v>34243</v>
       </c>
       <c r="E299" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -6980,7 +6977,7 @@
         <v>34608</v>
       </c>
       <c r="E300" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -6997,7 +6994,7 @@
         <v>34978</v>
       </c>
       <c r="E301" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -7014,7 +7011,7 @@
         <v>35348</v>
       </c>
       <c r="E302" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -7031,7 +7028,7 @@
         <v>35690</v>
       </c>
       <c r="E303" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -7048,7 +7045,7 @@
         <v>33147</v>
       </c>
       <c r="E304" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -7065,7 +7062,7 @@
         <v>33270</v>
       </c>
       <c r="E305" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
@@ -7082,7 +7079,7 @@
         <v>33543</v>
       </c>
       <c r="E306" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
@@ -7099,7 +7096,7 @@
         <v>32203</v>
       </c>
       <c r="E307" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
@@ -7116,7 +7113,7 @@
         <v>32568</v>
       </c>
       <c r="E308" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
@@ -7133,7 +7130,7 @@
         <v>32786</v>
       </c>
       <c r="E309" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
@@ -7150,7 +7147,7 @@
         <v>35004</v>
       </c>
       <c r="E310" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -7167,7 +7164,7 @@
         <v>35004</v>
       </c>
       <c r="E311" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
@@ -7184,7 +7181,7 @@
         <v>35612</v>
       </c>
       <c r="E312" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
@@ -7201,7 +7198,7 @@
         <v>35612</v>
       </c>
       <c r="E313" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
@@ -7218,7 +7215,7 @@
         <v>35612</v>
       </c>
       <c r="E314" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
@@ -7235,7 +7232,7 @@
         <v>35612</v>
       </c>
       <c r="E315" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Search and correct birth dates mistakes
</commit_message>
<xml_diff>
--- a/data/NewlyCreatedData/Checks/BirthDates.xlsx
+++ b/data/NewlyCreatedData/Checks/BirthDates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\monas\Git\repo\glt\GoldenLionTamarins\data\NewlyCreatedData\Checks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3146DBF7-37B8-470B-8E99-7490B70A3A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137A8EE5-1981-457C-9F62-CF380566361D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="488">
   <si>
     <t>Tatoo</t>
   </si>
@@ -1205,9 +1205,6 @@
     <t>01/04/95</t>
   </si>
   <si>
-    <t>00/01/00</t>
-  </si>
-  <si>
     <t>06/04/91</t>
   </si>
   <si>
@@ -1502,7 +1499,7 @@
     <t>01/07/97</t>
   </si>
   <si>
-    <t>BirthDMY</t>
+    <t>Birth_VR</t>
   </si>
 </sst>
 </file>
@@ -1871,7 +1868,7 @@
   <dimension ref="A1:E316"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,7 +1894,7 @@
         <v>352</v>
       </c>
       <c r="E1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2764,7 +2761,7 @@
         <v>353</v>
       </c>
       <c r="E52" t="s">
-        <v>389</v>
+        <v>353</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2781,7 +2778,7 @@
         <v>33334</v>
       </c>
       <c r="E53" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2798,7 +2795,7 @@
         <v>33482</v>
       </c>
       <c r="E54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2832,7 +2829,7 @@
         <v>35400</v>
       </c>
       <c r="E56" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2849,7 +2846,7 @@
         <v>35400</v>
       </c>
       <c r="E57" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2883,7 +2880,7 @@
         <v>36069</v>
       </c>
       <c r="E59" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2900,7 +2897,7 @@
         <v>36069</v>
       </c>
       <c r="E60" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2917,7 +2914,7 @@
         <v>36434</v>
       </c>
       <c r="E61" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2934,7 +2931,7 @@
         <v>36434</v>
       </c>
       <c r="E62" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2951,7 +2948,7 @@
         <v>33756</v>
       </c>
       <c r="E63" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2968,7 +2965,7 @@
         <v>31625</v>
       </c>
       <c r="E64" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2985,7 +2982,7 @@
         <v>224</v>
       </c>
       <c r="E65" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3002,7 +2999,7 @@
         <v>36708</v>
       </c>
       <c r="E66" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3019,7 +3016,7 @@
         <v>34608</v>
       </c>
       <c r="E67" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3036,7 +3033,7 @@
         <v>34608</v>
       </c>
       <c r="E68" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3053,7 +3050,7 @@
         <v>35004</v>
       </c>
       <c r="E69" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3070,7 +3067,7 @@
         <v>35004</v>
       </c>
       <c r="E70" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3087,7 +3084,7 @@
         <v>35309</v>
       </c>
       <c r="E71" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3104,7 +3101,7 @@
         <v>35309</v>
       </c>
       <c r="E72" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3121,7 +3118,7 @@
         <v>35674</v>
       </c>
       <c r="E73" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3138,7 +3135,7 @@
         <v>35674</v>
       </c>
       <c r="E74" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3155,7 +3152,7 @@
         <v>36130</v>
       </c>
       <c r="E75" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3172,7 +3169,7 @@
         <v>36130</v>
       </c>
       <c r="E76" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3189,7 +3186,7 @@
         <v>36434</v>
       </c>
       <c r="E77" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3206,7 +3203,7 @@
         <v>36434</v>
       </c>
       <c r="E78" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3257,7 +3254,7 @@
         <v>37165</v>
       </c>
       <c r="E81" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3274,7 +3271,7 @@
         <v>37165</v>
       </c>
       <c r="E82" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3291,7 +3288,7 @@
         <v>33270</v>
       </c>
       <c r="E83" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3308,7 +3305,7 @@
         <v>33329</v>
       </c>
       <c r="E84" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3325,7 +3322,7 @@
         <v>33329</v>
       </c>
       <c r="E85" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3342,7 +3339,7 @@
         <v>36272</v>
       </c>
       <c r="E86" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3410,7 +3407,7 @@
         <v>37165</v>
       </c>
       <c r="E90" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3427,7 +3424,7 @@
         <v>37165</v>
       </c>
       <c r="E91" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3461,7 +3458,7 @@
         <v>32721</v>
       </c>
       <c r="E93" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3512,7 +3509,7 @@
         <v>36495</v>
       </c>
       <c r="E96" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3529,7 +3526,7 @@
         <v>36495</v>
       </c>
       <c r="E97" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3563,7 +3560,7 @@
         <v>31822</v>
       </c>
       <c r="E99" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3580,7 +3577,7 @@
         <v>33520</v>
       </c>
       <c r="E100" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3597,7 +3594,7 @@
         <v>34020</v>
       </c>
       <c r="E101" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3614,7 +3611,7 @@
         <v>34020</v>
       </c>
       <c r="E102" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3631,7 +3628,7 @@
         <v>32478</v>
       </c>
       <c r="E103" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3648,7 +3645,7 @@
         <v>33158</v>
       </c>
       <c r="E104" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3665,7 +3662,7 @@
         <v>33158</v>
       </c>
       <c r="E105" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3682,7 +3679,7 @@
         <v>33520</v>
       </c>
       <c r="E106" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3699,7 +3696,7 @@
         <v>33257</v>
       </c>
       <c r="E107" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3716,7 +3713,7 @@
         <v>34608</v>
       </c>
       <c r="E108" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3801,7 +3798,7 @@
         <v>234</v>
       </c>
       <c r="E113" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3818,7 +3815,7 @@
         <v>234</v>
       </c>
       <c r="E114" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3886,7 +3883,7 @@
         <v>36100</v>
       </c>
       <c r="E118" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3903,7 +3900,7 @@
         <v>36100</v>
       </c>
       <c r="E119" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3954,7 +3951,7 @@
         <v>36708</v>
       </c>
       <c r="E122" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4005,7 +4002,7 @@
         <v>33628</v>
       </c>
       <c r="E125" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4022,7 +4019,7 @@
         <v>34001</v>
       </c>
       <c r="E126" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4039,7 +4036,7 @@
         <v>34608</v>
       </c>
       <c r="E127" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4056,7 +4053,7 @@
         <v>34608</v>
       </c>
       <c r="E128" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4073,7 +4070,7 @@
         <v>34881</v>
       </c>
       <c r="E129" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4107,7 +4104,7 @@
         <v>36708</v>
       </c>
       <c r="E131" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4124,7 +4121,7 @@
         <v>36708</v>
       </c>
       <c r="E132" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4141,7 +4138,7 @@
         <v>34881</v>
       </c>
       <c r="E133" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4158,7 +4155,7 @@
         <v>34881</v>
       </c>
       <c r="E134" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4175,7 +4172,7 @@
         <v>34881</v>
       </c>
       <c r="E135" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4192,7 +4189,7 @@
         <v>35278</v>
       </c>
       <c r="E136" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4209,7 +4206,7 @@
         <v>35643</v>
       </c>
       <c r="E137" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4226,7 +4223,7 @@
         <v>35643</v>
       </c>
       <c r="E138" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4243,7 +4240,7 @@
         <v>35643</v>
       </c>
       <c r="E139" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4345,7 +4342,7 @@
         <v>35348</v>
       </c>
       <c r="E145" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4362,7 +4359,7 @@
         <v>35348</v>
       </c>
       <c r="E146" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4379,7 +4376,7 @@
         <v>35711</v>
       </c>
       <c r="E147" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4396,7 +4393,7 @@
         <v>35711</v>
       </c>
       <c r="E148" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4413,7 +4410,7 @@
         <v>36065</v>
       </c>
       <c r="E149" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4430,7 +4427,7 @@
         <v>36065</v>
       </c>
       <c r="E150" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4447,7 +4444,7 @@
         <v>36413</v>
       </c>
       <c r="E151" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4464,7 +4461,7 @@
         <v>36413</v>
       </c>
       <c r="E152" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4549,7 +4546,7 @@
         <v>37165</v>
       </c>
       <c r="E157" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4566,7 +4563,7 @@
         <v>37165</v>
       </c>
       <c r="E158" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4583,7 +4580,7 @@
         <v>34339</v>
       </c>
       <c r="E159" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4600,7 +4597,7 @@
         <v>34339</v>
       </c>
       <c r="E160" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4617,7 +4614,7 @@
         <v>34620</v>
       </c>
       <c r="E161" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4668,7 +4665,7 @@
         <v>36404</v>
       </c>
       <c r="E164" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4685,7 +4682,7 @@
         <v>36557</v>
       </c>
       <c r="E165" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -4702,7 +4699,7 @@
         <v>36557</v>
       </c>
       <c r="E166" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4753,7 +4750,7 @@
         <v>37165</v>
       </c>
       <c r="E169" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4770,7 +4767,7 @@
         <v>37165</v>
       </c>
       <c r="E170" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4804,7 +4801,7 @@
         <v>34972</v>
       </c>
       <c r="E172" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4821,7 +4818,7 @@
         <v>34972</v>
       </c>
       <c r="E173" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4838,7 +4835,7 @@
         <v>35734</v>
       </c>
       <c r="E174" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4855,7 +4852,7 @@
         <v>35704</v>
       </c>
       <c r="E175" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4872,7 +4869,7 @@
         <v>36039</v>
       </c>
       <c r="E176" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -4889,7 +4886,7 @@
         <v>36039</v>
       </c>
       <c r="E177" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4906,7 +4903,7 @@
         <v>36404</v>
       </c>
       <c r="E178" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -4957,7 +4954,7 @@
         <v>33909</v>
       </c>
       <c r="E181" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -4974,7 +4971,7 @@
         <v>33140</v>
       </c>
       <c r="E182" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5008,7 +5005,7 @@
         <v>36178</v>
       </c>
       <c r="E184" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5025,7 +5022,7 @@
         <v>36178</v>
       </c>
       <c r="E185" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -5042,7 +5039,7 @@
         <v>181</v>
       </c>
       <c r="E186" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5059,7 +5056,7 @@
         <v>181</v>
       </c>
       <c r="E187" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -5127,7 +5124,7 @@
         <v>36923</v>
       </c>
       <c r="E191" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5144,7 +5141,7 @@
         <v>36923</v>
       </c>
       <c r="E192" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5161,7 +5158,7 @@
         <v>33695</v>
       </c>
       <c r="E193" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5178,7 +5175,7 @@
         <v>35217</v>
       </c>
       <c r="E194" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -5195,7 +5192,7 @@
         <v>35217</v>
       </c>
       <c r="E195" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5212,7 +5209,7 @@
         <v>35519</v>
       </c>
       <c r="E196" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -5229,7 +5226,7 @@
         <v>35519</v>
       </c>
       <c r="E197" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -5246,7 +5243,7 @@
         <v>36045</v>
       </c>
       <c r="E198" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -5263,7 +5260,7 @@
         <v>36045</v>
       </c>
       <c r="E199" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -5280,7 +5277,7 @@
         <v>36045</v>
       </c>
       <c r="E200" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5297,7 +5294,7 @@
         <v>36045</v>
       </c>
       <c r="E201" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -5314,7 +5311,7 @@
         <v>36045</v>
       </c>
       <c r="E202" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5331,7 +5328,7 @@
         <v>36178</v>
       </c>
       <c r="E203" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5348,7 +5345,7 @@
         <v>31472</v>
       </c>
       <c r="E204" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5365,7 +5362,7 @@
         <v>32118</v>
       </c>
       <c r="E205" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -5382,7 +5379,7 @@
         <v>37012</v>
       </c>
       <c r="E206" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -5399,7 +5396,7 @@
         <v>37012</v>
       </c>
       <c r="E207" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5416,7 +5413,7 @@
         <v>35777</v>
       </c>
       <c r="E208" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5433,7 +5430,7 @@
         <v>36069</v>
       </c>
       <c r="E209" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5450,7 +5447,7 @@
         <v>36069</v>
       </c>
       <c r="E210" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5467,7 +5464,7 @@
         <v>36404</v>
       </c>
       <c r="E211" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -5484,7 +5481,7 @@
         <v>36404</v>
       </c>
       <c r="E212" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -5535,7 +5532,7 @@
         <v>32174</v>
       </c>
       <c r="E215" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -5569,7 +5566,7 @@
         <v>35035</v>
       </c>
       <c r="E217" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -5586,7 +5583,7 @@
         <v>35035</v>
       </c>
       <c r="E218" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5603,7 +5600,7 @@
         <v>35462</v>
       </c>
       <c r="E219" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -5620,7 +5617,7 @@
         <v>35462</v>
       </c>
       <c r="E220" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -5654,7 +5651,7 @@
         <v>37165</v>
       </c>
       <c r="E222" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5671,7 +5668,7 @@
         <v>37165</v>
       </c>
       <c r="E223" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5688,7 +5685,7 @@
         <v>32752</v>
       </c>
       <c r="E224" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -5705,7 +5702,7 @@
         <v>32752</v>
       </c>
       <c r="E225" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -5722,7 +5719,7 @@
         <v>33899</v>
       </c>
       <c r="E226" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -5739,7 +5736,7 @@
         <v>31423</v>
       </c>
       <c r="E227" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -5756,7 +5753,7 @@
         <v>31423</v>
       </c>
       <c r="E228" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -5773,7 +5770,7 @@
         <v>36065</v>
       </c>
       <c r="E229" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -5790,7 +5787,7 @@
         <v>156</v>
       </c>
       <c r="E230" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -5841,7 +5838,7 @@
         <v>36065</v>
       </c>
       <c r="E233" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -5858,7 +5855,7 @@
         <v>36192</v>
       </c>
       <c r="E234" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -5875,7 +5872,7 @@
         <v>36192</v>
       </c>
       <c r="E235" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -5892,7 +5889,7 @@
         <v>36443</v>
       </c>
       <c r="E236" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -5909,7 +5906,7 @@
         <v>36443</v>
       </c>
       <c r="E237" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -5926,7 +5923,7 @@
         <v>36443</v>
       </c>
       <c r="E238" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -5943,7 +5940,7 @@
         <v>36443</v>
       </c>
       <c r="E239" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -5960,7 +5957,7 @@
         <v>156</v>
       </c>
       <c r="E240" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -5977,7 +5974,7 @@
         <v>156</v>
       </c>
       <c r="E241" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6028,7 +6025,7 @@
         <v>32478</v>
       </c>
       <c r="E244" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6045,7 +6042,7 @@
         <v>31321</v>
       </c>
       <c r="E245" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6062,7 +6059,7 @@
         <v>300</v>
       </c>
       <c r="E246" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6079,7 +6076,7 @@
         <v>300</v>
       </c>
       <c r="E247" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -6130,7 +6127,7 @@
         <v>298</v>
       </c>
       <c r="E250" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6147,7 +6144,7 @@
         <v>304</v>
       </c>
       <c r="E251" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -6164,7 +6161,7 @@
         <v>304</v>
       </c>
       <c r="E252" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -6181,7 +6178,7 @@
         <v>306</v>
       </c>
       <c r="E253" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6198,7 +6195,7 @@
         <v>306</v>
       </c>
       <c r="E254" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -6215,7 +6212,7 @@
         <v>306</v>
       </c>
       <c r="E255" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -6232,7 +6229,7 @@
         <v>306</v>
       </c>
       <c r="E256" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -6249,7 +6246,7 @@
         <v>33878</v>
       </c>
       <c r="E257" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6266,7 +6263,7 @@
         <v>34274</v>
       </c>
       <c r="E258" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -6283,7 +6280,7 @@
         <v>34759</v>
       </c>
       <c r="E259" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6300,7 +6297,7 @@
         <v>34992</v>
       </c>
       <c r="E260" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6317,7 +6314,7 @@
         <v>34992</v>
       </c>
       <c r="E261" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -6334,7 +6331,7 @@
         <v>35342</v>
       </c>
       <c r="E262" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -6351,7 +6348,7 @@
         <v>35342</v>
       </c>
       <c r="E263" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6368,7 +6365,7 @@
         <v>35499</v>
       </c>
       <c r="E264" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -6385,7 +6382,7 @@
         <v>35499</v>
       </c>
       <c r="E265" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -6402,7 +6399,7 @@
         <v>35713</v>
       </c>
       <c r="E266" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -6419,7 +6416,7 @@
         <v>35844</v>
       </c>
       <c r="E267" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -6436,7 +6433,7 @@
         <v>36089</v>
       </c>
       <c r="E268" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -6453,7 +6450,7 @@
         <v>36089</v>
       </c>
       <c r="E269" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -6470,7 +6467,7 @@
         <v>36130</v>
       </c>
       <c r="E270" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6487,7 +6484,7 @@
         <v>36130</v>
       </c>
       <c r="E271" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -6504,7 +6501,7 @@
         <v>36451</v>
       </c>
       <c r="E272" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -6521,7 +6518,7 @@
         <v>36434</v>
       </c>
       <c r="E273" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -6555,7 +6552,7 @@
         <v>33420</v>
       </c>
       <c r="E275" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
@@ -6589,7 +6586,7 @@
         <v>36861</v>
       </c>
       <c r="E277" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -6606,7 +6603,7 @@
         <v>36861</v>
       </c>
       <c r="E278" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -6623,7 +6620,7 @@
         <v>37135</v>
       </c>
       <c r="E279" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
@@ -6640,7 +6637,7 @@
         <v>37165</v>
       </c>
       <c r="E280" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
@@ -6657,7 +6654,7 @@
         <v>37165</v>
       </c>
       <c r="E281" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -6674,7 +6671,7 @@
         <v>34045</v>
       </c>
       <c r="E282" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -6691,7 +6688,7 @@
         <v>34045</v>
       </c>
       <c r="E283" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -6725,7 +6722,7 @@
         <v>33298</v>
       </c>
       <c r="E285" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -6776,7 +6773,7 @@
         <v>34243</v>
       </c>
       <c r="E288" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
@@ -6810,7 +6807,7 @@
         <v>35823</v>
       </c>
       <c r="E290" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -6827,7 +6824,7 @@
         <v>36066</v>
       </c>
       <c r="E291" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -6844,7 +6841,7 @@
         <v>36066</v>
       </c>
       <c r="E292" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -6861,7 +6858,7 @@
         <v>36404</v>
       </c>
       <c r="E293" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -6878,7 +6875,7 @@
         <v>36557</v>
       </c>
       <c r="E294" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -6895,7 +6892,7 @@
         <v>36557</v>
       </c>
       <c r="E295" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -6912,7 +6909,7 @@
         <v>36861</v>
       </c>
       <c r="E296" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -6929,7 +6926,7 @@
         <v>36861</v>
       </c>
       <c r="E297" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
@@ -6946,7 +6943,7 @@
         <v>37196</v>
       </c>
       <c r="E298" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -6963,7 +6960,7 @@
         <v>34243</v>
       </c>
       <c r="E299" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -6980,7 +6977,7 @@
         <v>34608</v>
       </c>
       <c r="E300" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -6997,7 +6994,7 @@
         <v>34978</v>
       </c>
       <c r="E301" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -7014,7 +7011,7 @@
         <v>35348</v>
       </c>
       <c r="E302" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -7031,7 +7028,7 @@
         <v>35690</v>
       </c>
       <c r="E303" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -7048,7 +7045,7 @@
         <v>33147</v>
       </c>
       <c r="E304" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -7065,7 +7062,7 @@
         <v>33270</v>
       </c>
       <c r="E305" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
@@ -7082,7 +7079,7 @@
         <v>33543</v>
       </c>
       <c r="E306" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
@@ -7099,7 +7096,7 @@
         <v>32203</v>
       </c>
       <c r="E307" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
@@ -7116,7 +7113,7 @@
         <v>32568</v>
       </c>
       <c r="E308" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
@@ -7133,7 +7130,7 @@
         <v>32786</v>
       </c>
       <c r="E309" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
@@ -7150,7 +7147,7 @@
         <v>35004</v>
       </c>
       <c r="E310" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -7167,7 +7164,7 @@
         <v>35004</v>
       </c>
       <c r="E311" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
@@ -7184,7 +7181,7 @@
         <v>35612</v>
       </c>
       <c r="E312" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
@@ -7201,7 +7198,7 @@
         <v>35612</v>
       </c>
       <c r="E313" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
@@ -7218,7 +7215,7 @@
         <v>35612</v>
       </c>
       <c r="E314" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
@@ -7235,7 +7232,7 @@
         <v>35612</v>
       </c>
       <c r="E315" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>